<commit_message>
Scenarij i tok događaja za rezervaciju sale.
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/PocetnaKonfiguracija.xlsx
+++ b/UseCaseIScenarij/PocetnaKonfiguracija.xlsx
@@ -59,9 +59,6 @@
     <t>Proširenja/alternative</t>
   </si>
   <si>
-    <t>Na osnovu podataka koje unese administrator formira se baza podataka o prostorijama na fakultetu, te se kreiraju korisnički računi za osoblje</t>
-  </si>
-  <si>
     <t>Administrator želi postaviti početne postavke sistema</t>
   </si>
   <si>
@@ -81,6 +78,11 @@
   </si>
   <si>
     <t>Tok događaja je pokriven podslučajevima</t>
+  </si>
+  <si>
+    <t>Na osnovu podataka koje unese administrator 
+formira se baza podataka o prostorijama 
+na fakultetu, te se kreiraju korisnički računi za osoblje</t>
   </si>
 </sst>
 </file>
@@ -114,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -122,19 +124,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -145,6 +332,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:B10"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Naziv" dataDxfId="2"/>
+    <tableColumn id="2" name="Početna konfiguracija" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,98 +645,98 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="30.19921875" customWidth="1"/>
-    <col min="2" max="2" width="67.1328125" customWidth="1"/>
+    <col min="2" max="2" width="44.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
+      <c r="B10" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -551,5 +749,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>